<commit_message>
Fix some issues in style and validation
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportPointSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportPointSampleFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBE7F836-83FB-40B7-8F5D-37FCCC70CE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A760E5D-B775-4640-AE39-189D547D0F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Trip Reference*</t>
   </si>
@@ -46,19 +47,25 @@
     <t>Pickup</t>
   </si>
   <si>
-    <t>testT</t>
-  </si>
-  <si>
-    <t>recT</t>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>sender11</t>
   </si>
   <si>
     <t>Dropoff</t>
   </si>
   <si>
-    <t>testR</t>
-  </si>
-  <si>
-    <t>recR</t>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>mem</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>rec12</t>
   </si>
 </sst>
 </file>
@@ -410,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -442,7 +449,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -459,7 +466,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -472,6 +479,23 @@
       </c>
       <c r="E3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>